<commit_message>
testdata.xlsx file for excel
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\git\repository2\KGF2\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E835E6D-71F6-46AE-B7D7-55CA20288240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5386A20C-D0FC-4592-9AC3-9C87FE9978E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13848" windowHeight="5748" activeTab="2" xr2:uid="{C34F22EE-B7AE-468F-A395-D304FBBEC72A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13848" windowHeight="5748" activeTab="3" xr2:uid="{C34F22EE-B7AE-468F-A395-D304FBBEC72A}"/>
   </bookViews>
   <sheets>
     <sheet name="TC001" sheetId="1" r:id="rId1"/>
     <sheet name="TC002" sheetId="2" r:id="rId2"/>
     <sheet name="Multiple" sheetId="4" r:id="rId3"/>
+    <sheet name="Reg" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>password</t>
   </si>
@@ -81,13 +82,52 @@
   </si>
   <si>
     <t>mahibh</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ActualUrl</t>
+  </si>
+  <si>
+    <t>canikissyoudarling23@gmail.com</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Testing@123</t>
+  </si>
+  <si>
+    <t>bh</t>
+  </si>
+  <si>
+    <t>https://shop-global.malaicha.com/registration-success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +195,22 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -201,10 +257,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -229,8 +286,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14476157-6169-47E7-BBAD-18F159D183F1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,18 +738,18 @@
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -700,4 +764,86 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0572F5-3FE8-4890-BD6A-A1CFAC233934}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6">
+        <v>91</v>
+      </c>
+      <c r="F2" s="6">
+        <v>9066678326</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2B22733C-FB66-4896-A54B-9FD308DEDF2A}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{84BCE28E-68AD-4BA9-8F49-61BB7892702E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>